<commit_message>
verify add works. Foreach loop does not work.
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>url</t>
   </si>
@@ -48,10 +48,6 @@
     <t>targetRent</t>
   </si>
   <si>
-    <t>newAddress</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>suburb</t>
   </si>
   <si>
@@ -83,15 +79,25 @@
     <t>http://new-keys.azurewebsites.net/PropertyOwners</t>
   </si>
   <si>
-    <t>aaa</t>
+    <t>golf</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>bbb</t>
+    <t>NewPropertyNameByRocky</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>golf</t>
+    <t>NewPropertyDescription</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Botany Road</t>
+  </si>
+  <si>
+    <t>Auckland</t>
+  </si>
+  <si>
+    <t>address</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -453,13 +459,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -476,7 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -504,19 +510,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.375" customWidth="1"/>
+    <col min="3" max="3" width="21.125" customWidth="1"/>
     <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.75" customWidth="1"/>
     <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.875" bestFit="1" customWidth="1"/>
@@ -539,30 +545,30 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -574,10 +580,10 @@
         <v>123</v>
       </c>
       <c r="E2">
-        <v>456</v>
+        <v>238</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2">
         <v>2011</v>
@@ -593,6 +599,21 @@
       </c>
       <c r="K2">
         <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>